<commit_message>
Smoke UI + API finalisée & CI standard mise en place
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47129D6-7B21-4D3E-AB5C-62608CFB6C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1269B6E7-D914-478A-B900-02975B4C2659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
   <sheets>
     <sheet name="cas_de_tests" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="309">
   <si>
     <t>CT-ID</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Bug</t>
-  </si>
-  <si>
-    <t>Evidence</t>
   </si>
   <si>
     <t>Commentaire</t>
@@ -102,12 +99,6 @@
   </si>
   <si>
     <t>CT-API-002.png</t>
-  </si>
-  <si>
-    <t>CT-LOGIN-002</t>
-  </si>
-  <si>
-    <t>CT-LOGIN-002.png</t>
   </si>
   <si>
     <t>CT-SIGNUP-001</t>
@@ -1196,6 +1187,21 @@
   </si>
   <si>
     <t>BUG-001</t>
+  </si>
+  <si>
+    <t>CT-AUTH-002</t>
+  </si>
+  <si>
+    <t>CT-AUTH-002.png</t>
+  </si>
+  <si>
+    <t>Preuve</t>
+  </si>
+  <si>
+    <t>La page "products" s'affiche
+La liste des produits est visible
+Aucun message d'erreur  / mauvaise redirection
+Aucun comportement inattendu n'est observé</t>
   </si>
 </sst>
 </file>
@@ -2040,11 +2046,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}">
-  <sheetPr codeName="Feuil1" filterMode="1"/>
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,1219 +2071,1213 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H2" t="s">
+        <v>296</v>
+      </c>
+      <c r="I2" t="s">
         <v>299</v>
       </c>
-      <c r="I2" t="s">
-        <v>302</v>
-      </c>
       <c r="J2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H3" t="s">
+        <v>296</v>
+      </c>
+      <c r="I3" t="s">
         <v>299</v>
       </c>
-      <c r="I3" t="s">
-        <v>302</v>
-      </c>
       <c r="J3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
+        <v>296</v>
+      </c>
+      <c r="I4" t="s">
         <v>299</v>
       </c>
-      <c r="I4" t="s">
-        <v>302</v>
-      </c>
       <c r="J4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H5" t="s">
+        <v>296</v>
+      </c>
+      <c r="I5" t="s">
         <v>299</v>
       </c>
-      <c r="I5" t="s">
-        <v>302</v>
-      </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>305</v>
       </c>
       <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G6" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="H6" t="s">
+        <v>296</v>
+      </c>
+      <c r="I6" t="s">
+        <v>299</v>
+      </c>
+      <c r="J6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" t="s">
         <v>93</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="G6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H6" t="s">
-        <v>299</v>
-      </c>
-      <c r="I6" t="s">
-        <v>302</v>
-      </c>
-      <c r="J6" t="s">
-        <v>107</v>
-      </c>
-      <c r="K6" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I7" t="s">
+        <v>299</v>
+      </c>
+      <c r="J7" t="s">
         <v>104</v>
       </c>
-      <c r="D7" t="s">
+      <c r="K7" t="s">
         <v>105</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G7" t="s">
-        <v>95</v>
-      </c>
-      <c r="H7" t="s">
-        <v>299</v>
-      </c>
-      <c r="I7" t="s">
-        <v>302</v>
-      </c>
-      <c r="J7" t="s">
-        <v>107</v>
-      </c>
-      <c r="K7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" t="s">
+        <v>296</v>
+      </c>
+      <c r="I8" t="s">
+        <v>299</v>
+      </c>
+      <c r="J8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" t="s">
         <v>131</v>
-      </c>
-      <c r="D8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G8" t="s">
-        <v>95</v>
-      </c>
-      <c r="H8" t="s">
-        <v>299</v>
-      </c>
-      <c r="I8" t="s">
-        <v>302</v>
-      </c>
-      <c r="J8" t="s">
-        <v>107</v>
-      </c>
-      <c r="K8" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" t="s">
+        <v>296</v>
+      </c>
+      <c r="I9" t="s">
+        <v>299</v>
+      </c>
+      <c r="J9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="C10" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="G9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="D10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" t="s">
+        <v>296</v>
+      </c>
+      <c r="I10" t="s">
         <v>299</v>
       </c>
-      <c r="I9" t="s">
-        <v>302</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="s">
         <v>107</v>
       </c>
-      <c r="K9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" t="s">
+        <v>296</v>
+      </c>
+      <c r="I11" t="s">
+        <v>299</v>
+      </c>
+      <c r="J11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
         <v>111</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G10" t="s">
-        <v>95</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" t="s">
+        <v>296</v>
+      </c>
+      <c r="I12" t="s">
         <v>299</v>
       </c>
-      <c r="I10" t="s">
-        <v>302</v>
-      </c>
-      <c r="J10" t="s">
-        <v>82</v>
-      </c>
-      <c r="K10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="J12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G13" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" t="s">
+        <v>296</v>
+      </c>
+      <c r="I13" t="s">
         <v>299</v>
       </c>
-      <c r="I11" t="s">
-        <v>302</v>
-      </c>
-      <c r="J11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G12" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="J13" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>275</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" t="s">
+        <v>296</v>
+      </c>
+      <c r="I14" t="s">
         <v>299</v>
       </c>
-      <c r="I12" t="s">
-        <v>302</v>
-      </c>
-      <c r="J12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G13" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="J14" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" t="s">
+        <v>296</v>
+      </c>
+      <c r="I15" t="s">
         <v>299</v>
       </c>
-      <c r="I13" t="s">
-        <v>302</v>
-      </c>
-      <c r="J13" t="s">
-        <v>119</v>
-      </c>
-      <c r="K13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>278</v>
-      </c>
-      <c r="C14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" t="s">
-        <v>272</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14" t="s">
-        <v>299</v>
-      </c>
-      <c r="I14" t="s">
-        <v>302</v>
-      </c>
-      <c r="J14" t="s">
-        <v>82</v>
-      </c>
-      <c r="K14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G15" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" t="s">
-        <v>299</v>
-      </c>
-      <c r="I15" t="s">
-        <v>302</v>
-      </c>
       <c r="J15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G16" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" t="s">
+        <v>296</v>
+      </c>
+      <c r="I16" t="s">
+        <v>299</v>
+      </c>
+      <c r="J16" t="s">
+        <v>104</v>
+      </c>
+      <c r="K16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
         <v>135</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="C17" t="s">
         <v>136</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="D17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G17" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I17" t="s">
         <v>299</v>
       </c>
-      <c r="I16" t="s">
-        <v>302</v>
-      </c>
-      <c r="J16" t="s">
-        <v>107</v>
-      </c>
-      <c r="K16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="J17" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" t="s">
         <v>138</v>
-      </c>
-      <c r="C17" t="s">
-        <v>139</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G17" t="s">
-        <v>95</v>
-      </c>
-      <c r="H17" t="s">
-        <v>299</v>
-      </c>
-      <c r="I17" t="s">
-        <v>302</v>
-      </c>
-      <c r="J17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K17" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" t="s">
+        <v>296</v>
+      </c>
+      <c r="I18" t="s">
+        <v>299</v>
+      </c>
+      <c r="J18" t="s">
+        <v>104</v>
+      </c>
+      <c r="K18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>45</v>
       </c>
-      <c r="B18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C18" t="s">
-        <v>143</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G18" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="B19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G19" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" t="s">
+        <v>296</v>
+      </c>
+      <c r="I19" t="s">
         <v>299</v>
       </c>
-      <c r="I18" t="s">
-        <v>302</v>
-      </c>
-      <c r="J18" t="s">
-        <v>107</v>
-      </c>
-      <c r="K18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>155</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="J19" t="s">
+        <v>79</v>
+      </c>
+      <c r="K19" t="s">
         <v>156</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G19" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" t="s">
+    </row>
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" t="s">
+        <v>296</v>
+      </c>
+      <c r="I20" t="s">
         <v>299</v>
       </c>
-      <c r="I19" t="s">
-        <v>302</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="J20" t="s">
+        <v>79</v>
+      </c>
+      <c r="K20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" t="s">
+        <v>296</v>
+      </c>
+      <c r="I21" t="s">
+        <v>299</v>
+      </c>
+      <c r="J21" t="s">
+        <v>79</v>
+      </c>
+      <c r="K21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" t="s">
+        <v>296</v>
+      </c>
+      <c r="I22" t="s">
+        <v>299</v>
+      </c>
+      <c r="J22" t="s">
+        <v>79</v>
+      </c>
+      <c r="K22" t="s">
         <v>82</v>
-      </c>
-      <c r="K19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="G20" t="s">
-        <v>95</v>
-      </c>
-      <c r="H20" t="s">
-        <v>299</v>
-      </c>
-      <c r="I20" t="s">
-        <v>302</v>
-      </c>
-      <c r="J20" t="s">
-        <v>82</v>
-      </c>
-      <c r="K20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" t="s">
-        <v>151</v>
-      </c>
-      <c r="C21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G21" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" t="s">
-        <v>299</v>
-      </c>
-      <c r="I21" t="s">
-        <v>302</v>
-      </c>
-      <c r="J21" t="s">
-        <v>82</v>
-      </c>
-      <c r="K21" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G22" t="s">
-        <v>95</v>
-      </c>
-      <c r="H22" t="s">
-        <v>299</v>
-      </c>
-      <c r="I22" t="s">
-        <v>302</v>
-      </c>
-      <c r="J22" t="s">
-        <v>82</v>
-      </c>
-      <c r="K22" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C23" t="s">
-        <v>148</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H23" t="s">
+        <v>296</v>
+      </c>
+      <c r="I23" t="s">
         <v>299</v>
       </c>
-      <c r="I23" t="s">
-        <v>302</v>
-      </c>
       <c r="J23" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C24" t="s">
-        <v>161</v>
-      </c>
-      <c r="D24" t="s">
-        <v>162</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G24" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H24" t="s">
+        <v>296</v>
+      </c>
+      <c r="I24" t="s">
         <v>299</v>
       </c>
-      <c r="I24" t="s">
-        <v>302</v>
-      </c>
       <c r="J24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K24" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H25" t="s">
+        <v>296</v>
+      </c>
+      <c r="I25" t="s">
         <v>299</v>
       </c>
-      <c r="I25" t="s">
-        <v>302</v>
-      </c>
       <c r="J25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K25" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H26" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" t="s">
+        <v>179</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C27" t="s">
-        <v>181</v>
-      </c>
-      <c r="D27" t="s">
-        <v>182</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G27" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H27" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G28" t="s">
+        <v>92</v>
+      </c>
+      <c r="H28" t="s">
+        <v>295</v>
+      </c>
+      <c r="I28" t="s">
         <v>167</v>
       </c>
-      <c r="C28" t="s">
-        <v>168</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G28" t="s">
-        <v>95</v>
-      </c>
-      <c r="H28" t="s">
-        <v>298</v>
-      </c>
-      <c r="I28" t="s">
-        <v>170</v>
-      </c>
       <c r="J28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K28" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29" t="s">
+        <v>182</v>
+      </c>
+      <c r="D29" t="s">
+        <v>183</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C29" t="s">
+      <c r="F29" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G29" t="s">
+        <v>92</v>
+      </c>
+      <c r="H29" t="s">
+        <v>295</v>
+      </c>
+      <c r="I29" t="s">
+        <v>167</v>
+      </c>
+      <c r="J29" t="s">
+        <v>104</v>
+      </c>
+      <c r="K29" t="s">
         <v>185</v>
-      </c>
-      <c r="D29" t="s">
-        <v>186</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G29" t="s">
-        <v>95</v>
-      </c>
-      <c r="H29" t="s">
-        <v>298</v>
-      </c>
-      <c r="I29" t="s">
-        <v>170</v>
-      </c>
-      <c r="J29" t="s">
-        <v>107</v>
-      </c>
-      <c r="K29" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H30" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I30" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K30" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" t="s">
+        <v>187</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C31" t="s">
+      <c r="F31" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G31" t="s">
+        <v>92</v>
+      </c>
+      <c r="H31" t="s">
+        <v>295</v>
+      </c>
+      <c r="I31" t="s">
+        <v>167</v>
+      </c>
+      <c r="J31" t="s">
+        <v>104</v>
+      </c>
+      <c r="K31" t="s">
         <v>190</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G31" t="s">
-        <v>95</v>
-      </c>
-      <c r="H31" t="s">
-        <v>298</v>
-      </c>
-      <c r="I31" t="s">
-        <v>170</v>
-      </c>
-      <c r="J31" t="s">
-        <v>107</v>
-      </c>
-      <c r="K31" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C32" t="s">
+      <c r="F32" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G32" t="s">
+        <v>92</v>
+      </c>
+      <c r="H32" t="s">
+        <v>295</v>
+      </c>
+      <c r="I32" t="s">
+        <v>167</v>
+      </c>
+      <c r="J32" t="s">
+        <v>104</v>
+      </c>
+      <c r="K32" t="s">
         <v>172</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G32" t="s">
-        <v>95</v>
-      </c>
-      <c r="H32" t="s">
-        <v>298</v>
-      </c>
-      <c r="I32" t="s">
-        <v>170</v>
-      </c>
-      <c r="J32" t="s">
-        <v>107</v>
-      </c>
-      <c r="K32" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C33" t="s">
+        <v>196</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G33" t="s">
+        <v>92</v>
+      </c>
+      <c r="H33" t="s">
+        <v>295</v>
+      </c>
+      <c r="I33" t="s">
+        <v>167</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C33" t="s">
+    </row>
+    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" t="s">
         <v>199</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="C34" t="s">
         <v>200</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="G33" t="s">
-        <v>95</v>
-      </c>
-      <c r="H33" t="s">
-        <v>298</v>
-      </c>
-      <c r="I33" t="s">
-        <v>170</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K33" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G34" t="s">
+        <v>92</v>
+      </c>
+      <c r="H34" t="s">
+        <v>295</v>
+      </c>
+      <c r="I34" t="s">
+        <v>167</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K34" s="1" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" t="s">
-        <v>202</v>
-      </c>
-      <c r="C34" t="s">
-        <v>203</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="G34" t="s">
-        <v>95</v>
-      </c>
-      <c r="H34" t="s">
-        <v>298</v>
-      </c>
-      <c r="I34" t="s">
-        <v>170</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G35" t="s">
+        <v>92</v>
+      </c>
+      <c r="H35" t="s">
+        <v>295</v>
+      </c>
+      <c r="I35" t="s">
+        <v>167</v>
+      </c>
+      <c r="J35" t="s">
+        <v>104</v>
+      </c>
+      <c r="K35" t="s">
         <v>176</v>
       </c>
-      <c r="C35" t="s">
-        <v>177</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="G35" t="s">
-        <v>95</v>
-      </c>
-      <c r="H35" t="s">
-        <v>298</v>
-      </c>
-      <c r="I35" t="s">
-        <v>170</v>
-      </c>
-      <c r="J35" t="s">
-        <v>107</v>
-      </c>
-      <c r="K35" t="s">
-        <v>179</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K35" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="M"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K35" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}"/>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:I4" xr:uid="{AD8D866F-2288-4C7D-9144-AB3ACAF95A3B}">
       <formula1>Type</formula1>
@@ -3304,8 +3304,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3322,7 +3322,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3340,1011 +3340,1011 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>307</v>
+      </c>
+      <c r="H1" t="s">
+        <v>278</v>
+      </c>
+      <c r="I1" t="s">
+        <v>279</v>
+      </c>
+      <c r="J1" t="s">
+        <v>280</v>
+      </c>
+      <c r="K1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" t="s">
-        <v>282</v>
-      </c>
-      <c r="J1" t="s">
-        <v>283</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>286</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
       </c>
       <c r="H2" s="2">
         <v>45993</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>283</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>286</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
       </c>
       <c r="H3" s="2">
         <v>45993</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>283</v>
+      </c>
+      <c r="G4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>286</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
       </c>
       <c r="H4" s="2">
         <v>45993</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>283</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>286</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="H5" s="2">
         <v>45993</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>283</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>286</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="H6" s="2">
         <v>45993</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J6" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>283</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>286</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="H7" s="2">
         <v>45994</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>283</v>
+      </c>
+      <c r="G8" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>286</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
       </c>
       <c r="H8" s="2">
         <v>45994</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>303</v>
+      </c>
+      <c r="B9" t="s">
+        <v>305</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>283</v>
+      </c>
+      <c r="G9" t="s">
         <v>306</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>286</v>
-      </c>
-      <c r="G9" t="s">
-        <v>23</v>
       </c>
       <c r="H9" s="2">
         <v>45994</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H10" s="2">
         <v>45994</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J10" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H11" s="2">
         <v>45994</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H12" s="2">
         <v>45994</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J12" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H13" s="2">
         <v>45994</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J13" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H14" s="2">
         <v>45995</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J14" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H15" s="2">
         <v>45995</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H16" s="2">
         <v>45995</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J16" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H17" s="2">
         <v>45995</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J17" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H18" s="2">
         <v>45995</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J18" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H19" s="2">
         <v>45995</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J19" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H20" s="2">
         <v>45995</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J20" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H21" s="2">
         <v>45995</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J21" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H22" s="2">
         <v>45995</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J22" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H23" s="2">
         <v>45995</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J23" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H24" s="2">
         <v>45995</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J24" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H25" s="2">
         <v>45995</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J25" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H26" s="2">
         <v>45995</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J26" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G27" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H27" s="2">
         <v>45995</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J27" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G28" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H28" s="2">
         <v>45995</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J28" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G29" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H29" s="2">
         <v>45995</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J29" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G30" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H30" s="2">
         <v>45995</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J30" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G31" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H31" s="2">
         <v>45995</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J31" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G32" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H32" s="2">
         <v>45995</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J32" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G33" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H33" s="2">
         <v>45995</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J33" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H34" s="2">
         <v>45995</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J34" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G35" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H35" s="2">
         <v>45995</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J35" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -4375,72 +4375,72 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test(regression) : ajouter de CT-CART-004 (EX-16)
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1269B6E7-D914-478A-B900-02975B4C2659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982E0988-DB0D-494D-AEC0-6FB8992961E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="310">
   <si>
     <t>CT-ID</t>
   </si>
@@ -1201,6 +1201,11 @@
     <t>La page "products" s'affiche
 La liste des produits est visible
 Aucun message d'erreur  / mauvaise redirection
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Le produit supprimé disparaît immédiatement de la liste
+Les autres produits restent inchangés
 Aucun comportement inattendu n'est observé</t>
   </si>
 </sst>
@@ -2046,11 +2051,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}">
-  <sheetPr codeName="Feuil1"/>
+  <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,7 +2141,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2171,7 +2176,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2235,7 +2240,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>305</v>
       </c>
@@ -2270,7 +2275,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2305,7 +2310,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2340,7 +2345,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -2410,7 +2415,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="44.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -2442,7 +2447,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2579,7 +2584,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2614,7 +2619,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2631,7 +2636,7 @@
         <v>137</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>232</v>
+        <v>309</v>
       </c>
       <c r="G17" t="s">
         <v>92</v>
@@ -2649,7 +2654,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2824,7 +2829,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -2859,7 +2864,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2894,7 +2899,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2964,7 +2969,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2996,7 +3001,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -3031,7 +3036,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -3066,7 +3071,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -3101,7 +3106,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -3136,7 +3141,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -3171,7 +3176,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -3206,7 +3211,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -3241,7 +3246,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -3277,7 +3282,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K35" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}"/>
+  <autoFilter ref="A1:K35" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="H"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:I4" xr:uid="{AD8D866F-2288-4C7D-9144-AB3ACAF95A3B}">
       <formula1>Type</formula1>

</xml_diff>

<commit_message>
test(regression) : ajouter de CT-CART-004 (EX-16) (#1)
Co-authored-by: Flavien Besnard <flavien.besnard2@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1269B6E7-D914-478A-B900-02975B4C2659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982E0988-DB0D-494D-AEC0-6FB8992961E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="310">
   <si>
     <t>CT-ID</t>
   </si>
@@ -1201,6 +1201,11 @@
     <t>La page "products" s'affiche
 La liste des produits est visible
 Aucun message d'erreur  / mauvaise redirection
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Le produit supprimé disparaît immédiatement de la liste
+Les autres produits restent inchangés
 Aucun comportement inattendu n'est observé</t>
   </si>
 </sst>
@@ -2046,11 +2051,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}">
-  <sheetPr codeName="Feuil1"/>
+  <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,7 +2141,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2171,7 +2176,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2235,7 +2240,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>305</v>
       </c>
@@ -2270,7 +2275,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2305,7 +2310,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2340,7 +2345,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -2410,7 +2415,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="44.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -2442,7 +2447,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2579,7 +2584,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2614,7 +2619,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2631,7 +2636,7 @@
         <v>137</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>232</v>
+        <v>309</v>
       </c>
       <c r="G17" t="s">
         <v>92</v>
@@ -2649,7 +2654,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2824,7 +2829,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -2859,7 +2864,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2894,7 +2899,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2964,7 +2969,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2996,7 +3001,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -3031,7 +3036,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -3066,7 +3071,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -3101,7 +3106,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -3136,7 +3141,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -3171,7 +3176,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -3206,7 +3211,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -3241,7 +3246,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -3277,7 +3282,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K35" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}"/>
+  <autoFilter ref="A1:K35" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="H"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:I4" xr:uid="{AD8D866F-2288-4C7D-9144-AB3ACAF95A3B}">
       <formula1>Type</formula1>

</xml_diff>

<commit_message>
test(CT-CART-002) : Total panier correct (EX-17) + fix google_vignette
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982E0988-DB0D-494D-AEC0-6FB8992961E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEDECFC-A658-40C5-B345-90831E50DB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
+    <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
   <sheets>
     <sheet name="cas_de_tests" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="311">
   <si>
     <t>CT-ID</t>
   </si>
@@ -1206,6 +1206,13 @@
   <si>
     <t>Le produit supprimé disparaît immédiatement de la liste
 Les autres produits restent inchangés
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Le nom du produit est affiché et non vide
+Le prix est affiché dans un format lisible (ex : Rs. 500)
+Des informations sur le produit sont visible (availability, condition,brand et notation)
+Une image du produit est visible
 Aucun comportement inattendu n'est observé</t>
   </si>
 </sst>
@@ -2054,8 +2061,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2397,7 +2404,7 @@
         <v>125</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>228</v>
+        <v>310</v>
       </c>
       <c r="G10" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
test(CT-CART-002) : Total panier correct (EX-17) + fix google_vignette (#2)
Co-authored-by: Flavien Besnard <flavien.besnard2@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982E0988-DB0D-494D-AEC0-6FB8992961E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEDECFC-A658-40C5-B345-90831E50DB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
+    <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
   <sheets>
     <sheet name="cas_de_tests" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="311">
   <si>
     <t>CT-ID</t>
   </si>
@@ -1206,6 +1206,13 @@
   <si>
     <t>Le produit supprimé disparaît immédiatement de la liste
 Les autres produits restent inchangés
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Le nom du produit est affiché et non vide
+Le prix est affiché dans un format lisible (ex : Rs. 500)
+Des informations sur le produit sont visible (availability, condition,brand et notation)
+Une image du produit est visible
 Aucun comportement inattendu n'est observé</t>
   </si>
 </sst>
@@ -2054,8 +2061,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2397,7 +2404,7 @@
         <v>125</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>228</v>
+        <v>310</v>
       </c>
       <c r="G10" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
test(CT-PRODUCTS-005): informations minimales fiche produit (EX-11)
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEDECFC-A658-40C5-B345-90831E50DB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6224E5-2438-42E6-BB45-50B1A51631BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -2061,8 +2061,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
test(CT-PRODUCTS-005): informations minimales fiche produit (EX-11) (#3)
Co-authored-by: Flavien Besnard <flavien.besnard2@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEDECFC-A658-40C5-B345-90831E50DB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6224E5-2438-42E6-BB45-50B1A51631BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -2061,8 +2061,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
test(CT-SIGNUP-001): Création compte valide (EX-04) + optimisation
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6224E5-2438-42E6-BB45-50B1A51631BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B92179-6885-43B5-9036-2A76CC6CFD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -2061,8 +2061,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Test/ct signup 001 creation compte valide (#4)
* test(CT-SIGNUP-001): Création compte valide (EX-04) + optimisation

* test(CT-SIGNUP-001): Création compte valide (EX-04) + optimisation

---------

Co-authored-by: Flavien Besnard <flavien.besnard2@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6224E5-2438-42E6-BB45-50B1A51631BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B92179-6885-43B5-9036-2A76CC6CFD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -2061,8 +2061,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
test(CT-CHECKOUT-003): adresse enregistré au checkout correcte + optimisation du signup
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B92179-6885-43B5-9036-2A76CC6CFD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9E7512-2166-4BE0-B571-2071E87F04ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="312">
   <si>
     <t>CT-ID</t>
   </si>
@@ -350,10 +350,6 @@
     <t>EX-03</t>
   </si>
   <si>
-    <t>1. L'utilisateur n'est pas connecté
-2. L'adresse email utilisée pour l'inscription n'existe pas encore dans le système</t>
-  </si>
-  <si>
     <t>Parcours heureux d'inscription</t>
   </si>
   <si>
@@ -1214,6 +1210,15 @@
 Des informations sur le produit sont visible (availability, condition,brand et notation)
 Une image du produit est visible
 Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Le compte est créé avec succès
+L'utilisateur est automatiquement connecté
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>1. L'utilisateur n'est pas connecté
+2. Adresse email unique</t>
   </si>
 </sst>
 </file>
@@ -2061,8 +2066,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,13 +2103,13 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J1" t="s">
         <v>60</v>
@@ -2121,31 +2126,31 @@
         <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>95</v>
+        <v>311</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>219</v>
+        <v>310</v>
       </c>
       <c r="G2" t="s">
         <v>92</v>
       </c>
       <c r="H2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J2" t="s">
         <v>79</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2153,34 +2158,34 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G3" t="s">
         <v>92</v>
       </c>
       <c r="H3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2188,31 +2193,31 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" t="s">
         <v>191</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G4" t="s">
         <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2226,22 +2231,22 @@
         <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G5" t="s">
         <v>92</v>
       </c>
       <c r="H5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J5" t="s">
         <v>79</v>
@@ -2249,7 +2254,7 @@
     </row>
     <row r="6" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B6" t="s">
         <v>88</v>
@@ -2264,19 +2269,19 @@
         <v>91</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G6" t="s">
         <v>92</v>
       </c>
       <c r="H6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K6" t="s">
         <v>93</v>
@@ -2287,34 +2292,34 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
         <v>100</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>101</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G7" t="s">
         <v>92</v>
       </c>
       <c r="H7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J7" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" t="s">
         <v>104</v>
-      </c>
-      <c r="K7" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -2322,34 +2327,34 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" t="s">
         <v>127</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>128</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G8" t="s">
         <v>92</v>
       </c>
       <c r="H8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -2357,34 +2362,34 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" t="s">
         <v>118</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G9" t="s">
         <v>92</v>
       </c>
       <c r="H9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2392,34 +2397,34 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
         <v>123</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D10" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G10" t="s">
         <v>92</v>
       </c>
       <c r="H10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J10" t="s">
         <v>79</v>
       </c>
       <c r="K10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="44.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2427,31 +2432,31 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" t="s">
         <v>106</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>107</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G11" t="s">
         <v>92</v>
       </c>
       <c r="H11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -2459,31 +2464,31 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
         <v>110</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G12" t="s">
         <v>92</v>
       </c>
       <c r="H12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -2491,34 +2496,34 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
         <v>113</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D13" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G13" t="s">
         <v>92</v>
       </c>
       <c r="H13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J13" t="s">
+        <v>115</v>
+      </c>
+      <c r="K13" t="s">
         <v>116</v>
-      </c>
-      <c r="K13" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2526,28 +2531,28 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C14" t="s">
         <v>71</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G14" t="s">
         <v>92</v>
       </c>
       <c r="H14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J14" t="s">
         <v>79</v>
@@ -2570,25 +2575,25 @@
         <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G15" t="s">
         <v>92</v>
       </c>
       <c r="H15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J15" t="s">
         <v>79</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2596,34 +2601,34 @@
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G16" t="s">
         <v>92</v>
       </c>
       <c r="H16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2631,34 +2636,34 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" t="s">
         <v>135</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G17" t="s">
         <v>92</v>
       </c>
       <c r="H17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J17" t="s">
         <v>79</v>
       </c>
       <c r="K17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2666,34 +2671,34 @@
         <v>42</v>
       </c>
       <c r="B18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" t="s">
         <v>139</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G18" t="s">
         <v>92</v>
       </c>
       <c r="H18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2701,34 +2706,34 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" t="s">
         <v>152</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G19" t="s">
         <v>92</v>
       </c>
       <c r="H19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J19" t="s">
         <v>79</v>
       </c>
       <c r="K19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2748,16 +2753,16 @@
         <v>76</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G20" t="s">
         <v>92</v>
       </c>
       <c r="H20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J20" t="s">
         <v>79</v>
@@ -2771,34 +2776,34 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C21" t="s">
         <v>74</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G21" t="s">
         <v>92</v>
       </c>
       <c r="H21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J21" t="s">
         <v>79</v>
       </c>
       <c r="K21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2818,16 +2823,16 @@
         <v>77</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G22" t="s">
         <v>92</v>
       </c>
       <c r="H22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J22" t="s">
         <v>79</v>
@@ -2841,34 +2846,34 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" t="s">
         <v>144</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G23" t="s">
         <v>92</v>
       </c>
       <c r="H23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2876,34 +2881,34 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" t="s">
         <v>157</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>158</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G24" t="s">
         <v>92</v>
       </c>
       <c r="H24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K24" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2911,34 +2916,34 @@
         <v>47</v>
       </c>
       <c r="B25" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" t="s">
         <v>161</v>
       </c>
-      <c r="C25" t="s">
-        <v>162</v>
-      </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G25" t="s">
         <v>92</v>
       </c>
       <c r="H25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2952,22 +2957,22 @@
         <v>83</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G26" t="s">
         <v>92</v>
       </c>
       <c r="H26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J26" t="s">
         <v>79</v>
@@ -2981,31 +2986,31 @@
         <v>51</v>
       </c>
       <c r="B27" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27" t="s">
         <v>177</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>178</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G27" t="s">
         <v>92</v>
       </c>
       <c r="H27" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3013,34 +3018,34 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" t="s">
         <v>164</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G28" t="s">
         <v>92</v>
       </c>
       <c r="H28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -3048,34 +3053,34 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" t="s">
         <v>181</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>182</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G29" t="s">
         <v>92</v>
       </c>
       <c r="H29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3089,28 +3094,28 @@
         <v>84</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G30" t="s">
         <v>92</v>
       </c>
       <c r="H30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -3118,34 +3123,34 @@
         <v>53</v>
       </c>
       <c r="B31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C31" t="s">
         <v>186</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G31" t="s">
         <v>92</v>
       </c>
       <c r="H31" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3153,34 +3158,34 @@
         <v>49</v>
       </c>
       <c r="B32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" t="s">
         <v>168</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G32" t="s">
         <v>92</v>
       </c>
       <c r="H32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3188,34 +3193,34 @@
         <v>54</v>
       </c>
       <c r="B33" t="s">
+        <v>194</v>
+      </c>
+      <c r="C33" t="s">
         <v>195</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G33" t="s">
         <v>92</v>
       </c>
       <c r="H33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3223,34 +3228,34 @@
         <v>55</v>
       </c>
       <c r="B34" t="s">
+        <v>198</v>
+      </c>
+      <c r="C34" t="s">
         <v>199</v>
       </c>
-      <c r="C34" t="s">
-        <v>200</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G34" t="s">
         <v>92</v>
       </c>
       <c r="H34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -3258,34 +3263,34 @@
         <v>50</v>
       </c>
       <c r="B35" t="s">
+        <v>172</v>
+      </c>
+      <c r="C35" t="s">
         <v>173</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G35" t="s">
         <v>92</v>
       </c>
       <c r="H35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -3340,7 +3345,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3358,16 +3363,16 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I1" t="s">
         <v>278</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>279</v>
-      </c>
-      <c r="J1" t="s">
-        <v>280</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
@@ -3375,19 +3380,19 @@
     </row>
     <row r="2" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -3396,27 +3401,27 @@
         <v>45993</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -3425,27 +3430,27 @@
         <v>45993</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
@@ -3454,27 +3459,27 @@
         <v>45993</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>14</v>
@@ -3483,27 +3488,27 @@
         <v>45993</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>16</v>
@@ -3512,27 +3517,27 @@
         <v>45993</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>18</v>
@@ -3541,27 +3546,27 @@
         <v>45994</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G8" t="s">
         <v>20</v>
@@ -3570,56 +3575,56 @@
         <v>45994</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H9" s="2">
         <v>45994</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>22</v>
@@ -3628,27 +3633,27 @@
         <v>45994</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -3657,27 +3662,27 @@
         <v>45994</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G12" t="s">
         <v>26</v>
@@ -3686,27 +3691,27 @@
         <v>45994</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B13" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>28</v>
@@ -3715,27 +3720,27 @@
         <v>45994</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B14" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>30</v>
@@ -3744,62 +3749,62 @@
         <v>45995</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H15" s="2">
         <v>45995</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G16" t="s">
         <v>34</v>
@@ -3808,27 +3813,27 @@
         <v>45995</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G17" t="s">
         <v>36</v>
@@ -3837,27 +3842,27 @@
         <v>45995</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G18" t="s">
         <v>38</v>
@@ -3866,503 +3871,503 @@
         <v>45995</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B19" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H19" s="2">
         <v>45995</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H20" s="2">
         <v>45995</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H21" s="2">
         <v>45995</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B22" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H22" s="2">
         <v>45995</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H23" s="2">
         <v>45995</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G24" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H24" s="2">
         <v>45995</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H25" s="2">
         <v>45995</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H26" s="2">
         <v>45995</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H27" s="2">
         <v>45995</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H28" s="2">
         <v>45995</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H29" s="2">
         <v>45995</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J29" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B30" t="s">
         <v>50</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H30" s="2">
         <v>45995</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B31" t="s">
         <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H31" s="2">
         <v>45995</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B32" t="s">
         <v>52</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H32" s="2">
         <v>45995</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B33" t="s">
         <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H33" s="2">
         <v>45995</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B34" t="s">
         <v>54</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H34" s="2">
         <v>45995</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B35" t="s">
         <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H35" s="2">
         <v>45995</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -4393,19 +4398,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" t="s">
         <v>291</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>292</v>
-      </c>
-      <c r="E1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4413,52 +4418,52 @@
         <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C2" t="s">
         <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test(CT-CHECKOUT-003): adresse checkout correcte + optimisation du signup (#5)
Co-authored-by: Flavien Besnard <flavien.besnard2@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B92179-6885-43B5-9036-2A76CC6CFD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9E7512-2166-4BE0-B571-2071E87F04ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="312">
   <si>
     <t>CT-ID</t>
   </si>
@@ -350,10 +350,6 @@
     <t>EX-03</t>
   </si>
   <si>
-    <t>1. L'utilisateur n'est pas connecté
-2. L'adresse email utilisée pour l'inscription n'existe pas encore dans le système</t>
-  </si>
-  <si>
     <t>Parcours heureux d'inscription</t>
   </si>
   <si>
@@ -1214,6 +1210,15 @@
 Des informations sur le produit sont visible (availability, condition,brand et notation)
 Une image du produit est visible
 Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Le compte est créé avec succès
+L'utilisateur est automatiquement connecté
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>1. L'utilisateur n'est pas connecté
+2. Adresse email unique</t>
   </si>
 </sst>
 </file>
@@ -2061,8 +2066,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,13 +2103,13 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J1" t="s">
         <v>60</v>
@@ -2121,31 +2126,31 @@
         <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>95</v>
+        <v>311</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>219</v>
+        <v>310</v>
       </c>
       <c r="G2" t="s">
         <v>92</v>
       </c>
       <c r="H2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J2" t="s">
         <v>79</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2153,34 +2158,34 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G3" t="s">
         <v>92</v>
       </c>
       <c r="H3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2188,31 +2193,31 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" t="s">
         <v>191</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G4" t="s">
         <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2226,22 +2231,22 @@
         <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G5" t="s">
         <v>92</v>
       </c>
       <c r="H5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J5" t="s">
         <v>79</v>
@@ -2249,7 +2254,7 @@
     </row>
     <row r="6" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B6" t="s">
         <v>88</v>
@@ -2264,19 +2269,19 @@
         <v>91</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G6" t="s">
         <v>92</v>
       </c>
       <c r="H6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K6" t="s">
         <v>93</v>
@@ -2287,34 +2292,34 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
         <v>100</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>101</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G7" t="s">
         <v>92</v>
       </c>
       <c r="H7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J7" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" t="s">
         <v>104</v>
-      </c>
-      <c r="K7" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -2322,34 +2327,34 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" t="s">
         <v>127</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>128</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G8" t="s">
         <v>92</v>
       </c>
       <c r="H8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -2357,34 +2362,34 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" t="s">
         <v>118</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G9" t="s">
         <v>92</v>
       </c>
       <c r="H9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2392,34 +2397,34 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
         <v>123</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D10" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G10" t="s">
         <v>92</v>
       </c>
       <c r="H10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J10" t="s">
         <v>79</v>
       </c>
       <c r="K10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="44.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2427,31 +2432,31 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" t="s">
         <v>106</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>107</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G11" t="s">
         <v>92</v>
       </c>
       <c r="H11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -2459,31 +2464,31 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
         <v>110</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G12" t="s">
         <v>92</v>
       </c>
       <c r="H12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -2491,34 +2496,34 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
         <v>113</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D13" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G13" t="s">
         <v>92</v>
       </c>
       <c r="H13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J13" t="s">
+        <v>115</v>
+      </c>
+      <c r="K13" t="s">
         <v>116</v>
-      </c>
-      <c r="K13" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2526,28 +2531,28 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C14" t="s">
         <v>71</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G14" t="s">
         <v>92</v>
       </c>
       <c r="H14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J14" t="s">
         <v>79</v>
@@ -2570,25 +2575,25 @@
         <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G15" t="s">
         <v>92</v>
       </c>
       <c r="H15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J15" t="s">
         <v>79</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2596,34 +2601,34 @@
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G16" t="s">
         <v>92</v>
       </c>
       <c r="H16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2631,34 +2636,34 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" t="s">
         <v>135</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G17" t="s">
         <v>92</v>
       </c>
       <c r="H17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J17" t="s">
         <v>79</v>
       </c>
       <c r="K17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2666,34 +2671,34 @@
         <v>42</v>
       </c>
       <c r="B18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" t="s">
         <v>139</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G18" t="s">
         <v>92</v>
       </c>
       <c r="H18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2701,34 +2706,34 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" t="s">
         <v>152</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G19" t="s">
         <v>92</v>
       </c>
       <c r="H19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J19" t="s">
         <v>79</v>
       </c>
       <c r="K19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2748,16 +2753,16 @@
         <v>76</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G20" t="s">
         <v>92</v>
       </c>
       <c r="H20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J20" t="s">
         <v>79</v>
@@ -2771,34 +2776,34 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C21" t="s">
         <v>74</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G21" t="s">
         <v>92</v>
       </c>
       <c r="H21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J21" t="s">
         <v>79</v>
       </c>
       <c r="K21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2818,16 +2823,16 @@
         <v>77</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G22" t="s">
         <v>92</v>
       </c>
       <c r="H22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J22" t="s">
         <v>79</v>
@@ -2841,34 +2846,34 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" t="s">
         <v>144</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G23" t="s">
         <v>92</v>
       </c>
       <c r="H23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2876,34 +2881,34 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" t="s">
         <v>157</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>158</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G24" t="s">
         <v>92</v>
       </c>
       <c r="H24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K24" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2911,34 +2916,34 @@
         <v>47</v>
       </c>
       <c r="B25" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" t="s">
         <v>161</v>
       </c>
-      <c r="C25" t="s">
-        <v>162</v>
-      </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G25" t="s">
         <v>92</v>
       </c>
       <c r="H25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2952,22 +2957,22 @@
         <v>83</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G26" t="s">
         <v>92</v>
       </c>
       <c r="H26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J26" t="s">
         <v>79</v>
@@ -2981,31 +2986,31 @@
         <v>51</v>
       </c>
       <c r="B27" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27" t="s">
         <v>177</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>178</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G27" t="s">
         <v>92</v>
       </c>
       <c r="H27" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3013,34 +3018,34 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" t="s">
         <v>164</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G28" t="s">
         <v>92</v>
       </c>
       <c r="H28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -3048,34 +3053,34 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" t="s">
         <v>181</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>182</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G29" t="s">
         <v>92</v>
       </c>
       <c r="H29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3089,28 +3094,28 @@
         <v>84</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G30" t="s">
         <v>92</v>
       </c>
       <c r="H30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -3118,34 +3123,34 @@
         <v>53</v>
       </c>
       <c r="B31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C31" t="s">
         <v>186</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G31" t="s">
         <v>92</v>
       </c>
       <c r="H31" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3153,34 +3158,34 @@
         <v>49</v>
       </c>
       <c r="B32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" t="s">
         <v>168</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G32" t="s">
         <v>92</v>
       </c>
       <c r="H32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3188,34 +3193,34 @@
         <v>54</v>
       </c>
       <c r="B33" t="s">
+        <v>194</v>
+      </c>
+      <c r="C33" t="s">
         <v>195</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G33" t="s">
         <v>92</v>
       </c>
       <c r="H33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3223,34 +3228,34 @@
         <v>55</v>
       </c>
       <c r="B34" t="s">
+        <v>198</v>
+      </c>
+      <c r="C34" t="s">
         <v>199</v>
       </c>
-      <c r="C34" t="s">
-        <v>200</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G34" t="s">
         <v>92</v>
       </c>
       <c r="H34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -3258,34 +3263,34 @@
         <v>50</v>
       </c>
       <c r="B35" t="s">
+        <v>172</v>
+      </c>
+      <c r="C35" t="s">
         <v>173</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G35" t="s">
         <v>92</v>
       </c>
       <c r="H35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -3340,7 +3345,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3358,16 +3363,16 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I1" t="s">
         <v>278</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>279</v>
-      </c>
-      <c r="J1" t="s">
-        <v>280</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
@@ -3375,19 +3380,19 @@
     </row>
     <row r="2" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -3396,27 +3401,27 @@
         <v>45993</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -3425,27 +3430,27 @@
         <v>45993</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
@@ -3454,27 +3459,27 @@
         <v>45993</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>14</v>
@@ -3483,27 +3488,27 @@
         <v>45993</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>16</v>
@@ -3512,27 +3517,27 @@
         <v>45993</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>18</v>
@@ -3541,27 +3546,27 @@
         <v>45994</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G8" t="s">
         <v>20</v>
@@ -3570,56 +3575,56 @@
         <v>45994</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H9" s="2">
         <v>45994</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>22</v>
@@ -3628,27 +3633,27 @@
         <v>45994</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -3657,27 +3662,27 @@
         <v>45994</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G12" t="s">
         <v>26</v>
@@ -3686,27 +3691,27 @@
         <v>45994</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B13" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>28</v>
@@ -3715,27 +3720,27 @@
         <v>45994</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B14" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>30</v>
@@ -3744,62 +3749,62 @@
         <v>45995</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H15" s="2">
         <v>45995</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G16" t="s">
         <v>34</v>
@@ -3808,27 +3813,27 @@
         <v>45995</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G17" t="s">
         <v>36</v>
@@ -3837,27 +3842,27 @@
         <v>45995</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G18" t="s">
         <v>38</v>
@@ -3866,503 +3871,503 @@
         <v>45995</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B19" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H19" s="2">
         <v>45995</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H20" s="2">
         <v>45995</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H21" s="2">
         <v>45995</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B22" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H22" s="2">
         <v>45995</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H23" s="2">
         <v>45995</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G24" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H24" s="2">
         <v>45995</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H25" s="2">
         <v>45995</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H26" s="2">
         <v>45995</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H27" s="2">
         <v>45995</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H28" s="2">
         <v>45995</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H29" s="2">
         <v>45995</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J29" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B30" t="s">
         <v>50</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H30" s="2">
         <v>45995</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B31" t="s">
         <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H31" s="2">
         <v>45995</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B32" t="s">
         <v>52</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H32" s="2">
         <v>45995</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B33" t="s">
         <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H33" s="2">
         <v>45995</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B34" t="s">
         <v>54</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H34" s="2">
         <v>45995</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B35" t="s">
         <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H35" s="2">
         <v>45995</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -4393,19 +4398,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" t="s">
         <v>291</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>292</v>
-      </c>
-      <c r="E1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4413,52 +4418,52 @@
         <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C2" t="s">
         <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test(CT-CHECKOUT-002): champ obligatoire avant paiement (card number) EX-20
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9E7512-2166-4BE0-B571-2071E87F04ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D9FC6B-78EC-46E0-9D19-4BC18F68DBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -2066,8 +2066,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3258,7 +3258,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
test(CT-CHECKOUT-002): champ obligatoire avant paiement (card number) EX-20 (#6)
Co-authored-by: Flavien Besnard <flavien.besnard2@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9E7512-2166-4BE0-B571-2071E87F04ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D9FC6B-78EC-46E0-9D19-4BC18F68DBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -2066,8 +2066,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3258,7 +3258,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
test(CT-PAYMENT-001): Paiement réussi et confirmation  EX-20
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D9FC6B-78EC-46E0-9D19-4BC18F68DBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BBEE78-2CE1-447E-A651-AFA8DC8FA2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -2066,8 +2066,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Test(CT-PAYMENT-001):  paiement reussi et confirmation commande (EX-20) (#7)
* test(CT-PAYMENT-001): Paiement réussi et confirmation  EX-20

* optimisation du readme

---------

Co-authored-by: Flavien Besnard <flavien.besnard2@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D9FC6B-78EC-46E0-9D19-4BC18F68DBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BBEE78-2CE1-447E-A651-AFA8DC8FA2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
@@ -2066,8 +2066,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
test(CT-API-008): Vérification login avec identifiants invalides verifyLogin EX-28
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BBEE78-2CE1-447E-A651-AFA8DC8FA2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB31911-C5C0-44D2-8167-469173FC0922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
   <sheets>
     <sheet name="cas_de_tests" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="322">
   <si>
     <t>CT-ID</t>
   </si>
@@ -1219,6 +1219,76 @@
   <si>
     <t>1. L'utilisateur n'est pas connecté
 2. Adresse email unique</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+Le JSON contient une liste non vide de marques
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+La réponse contient une structure JSON valide
+La liste des produits est présente et non vide (au moins 1 produit est retourné)
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+Body JSON : message = email demandé + information cohérente avec le compte
+Aucun message d'erreur n'est retourné
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode =  200
+Le JSON retournée contient au moins un produit correspondent
+Les produits retournés contiennent le mot clé dans leur name ou category
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 201
+Body JSON : message contient "User created"
+Le compte est bien créé
+Une seconde tentative avec le même email provoque un message de type "Email already exists"
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 404
+Body JSON : message contient "User not found"
+Aucun succès ni "User exists!" n'est retourné
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+Body JSON : message contient "User exists"
+l'API confirme seulement l'existence d'un user 
+Aucune connexon réelle n'est effectuée
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 400
+Body JSON : message contient "Bad request, search_product parameter is missing in POST request"
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+Body JSON : message contient "User updated" 
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+Body JSON : message contient "Account deleted"
+Si l'on retente une suppression avec le même email -&gt; message "Account not found"
+Aucun comportement inattendu n'est observé</t>
   </si>
 </sst>
 </file>
@@ -2063,11 +2133,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}">
-  <sheetPr codeName="Feuil1" filterMode="1"/>
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="E31" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2153,7 +2223,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2188,7 +2258,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2252,7 +2322,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>304</v>
       </c>
@@ -2287,7 +2357,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2322,7 +2392,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2357,7 +2427,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -2427,7 +2497,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="44.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -2459,7 +2529,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2491,7 +2561,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2596,7 +2666,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2666,7 +2736,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2841,7 +2911,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -2876,7 +2946,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2911,7 +2981,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2946,7 +3016,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -2963,7 +3033,7 @@
         <v>78</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>215</v>
+        <v>313</v>
       </c>
       <c r="G26" t="s">
         <v>92</v>
@@ -2981,7 +3051,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2998,7 +3068,7 @@
         <v>179</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>251</v>
+        <v>312</v>
       </c>
       <c r="G27" t="s">
         <v>92</v>
@@ -3013,7 +3083,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -3030,7 +3100,7 @@
         <v>165</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>245</v>
+        <v>315</v>
       </c>
       <c r="G28" t="s">
         <v>92</v>
@@ -3048,7 +3118,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -3065,7 +3135,7 @@
         <v>183</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>253</v>
+        <v>319</v>
       </c>
       <c r="G29" t="s">
         <v>92</v>
@@ -3083,7 +3153,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -3100,7 +3170,7 @@
         <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>216</v>
+        <v>318</v>
       </c>
       <c r="G30" t="s">
         <v>92</v>
@@ -3118,7 +3188,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -3135,7 +3205,7 @@
         <v>188</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>255</v>
+        <v>317</v>
       </c>
       <c r="G31" t="s">
         <v>92</v>
@@ -3153,7 +3223,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -3170,7 +3240,7 @@
         <v>170</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>247</v>
+        <v>316</v>
       </c>
       <c r="G32" t="s">
         <v>92</v>
@@ -3188,7 +3258,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -3205,7 +3275,7 @@
         <v>265</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>257</v>
+        <v>320</v>
       </c>
       <c r="G33" t="s">
         <v>92</v>
@@ -3223,7 +3293,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -3240,7 +3310,7 @@
         <v>266</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>259</v>
+        <v>314</v>
       </c>
       <c r="G34" t="s">
         <v>92</v>
@@ -3258,7 +3328,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -3275,7 +3345,7 @@
         <v>264</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>249</v>
+        <v>321</v>
       </c>
       <c r="G35" t="s">
         <v>92</v>
@@ -3294,13 +3364,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K35" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="H"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K35" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}"/>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:I4" xr:uid="{AD8D866F-2288-4C7D-9144-AB3ACAF95A3B}">
       <formula1>Type</formula1>

</xml_diff>

<commit_message>
test(CT-API-008): Vérification login avec identifiants invalides verifyLogin EX-28 (#9)
Co-authored-by: Flavien Besnard <flavien.besnard2@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/cas_de_tests.xlsx
+++ b/docs/cas_de_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testeur logiciel\qa-portfolio-automationexercise\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BBEE78-2CE1-447E-A651-AFA8DC8FA2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB31911-C5C0-44D2-8167-469173FC0922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-684" windowWidth="23256" windowHeight="12456" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{218A45A3-A2FB-47AD-BD45-4EB4C1AFFDD0}"/>
   </bookViews>
   <sheets>
     <sheet name="cas_de_tests" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="322">
   <si>
     <t>CT-ID</t>
   </si>
@@ -1219,6 +1219,76 @@
   <si>
     <t>1. L'utilisateur n'est pas connecté
 2. Adresse email unique</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+Le JSON contient une liste non vide de marques
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+La réponse contient une structure JSON valide
+La liste des produits est présente et non vide (au moins 1 produit est retourné)
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+Body JSON : message = email demandé + information cohérente avec le compte
+Aucun message d'erreur n'est retourné
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode =  200
+Le JSON retournée contient au moins un produit correspondent
+Les produits retournés contiennent le mot clé dans leur name ou category
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 201
+Body JSON : message contient "User created"
+Le compte est bien créé
+Une seconde tentative avec le même email provoque un message de type "Email already exists"
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 404
+Body JSON : message contient "User not found"
+Aucun succès ni "User exists!" n'est retourné
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+Body JSON : message contient "User exists"
+l'API confirme seulement l'existence d'un user 
+Aucune connexon réelle n'est effectuée
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 400
+Body JSON : message contient "Bad request, search_product parameter is missing in POST request"
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+Body JSON : message contient "User updated" 
+Aucun comportement inattendu n'est observé</t>
+  </si>
+  <si>
+    <t>Code HTTP = 200 (comportement de l'API)
+Body JSON : responseCode = 200
+Body JSON : message contient "Account deleted"
+Si l'on retente une suppression avec le même email -&gt; message "Account not found"
+Aucun comportement inattendu n'est observé</t>
   </si>
 </sst>
 </file>
@@ -2063,11 +2133,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}">
-  <sheetPr codeName="Feuil1" filterMode="1"/>
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="E31" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2153,7 +2223,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2188,7 +2258,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2252,7 +2322,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>304</v>
       </c>
@@ -2287,7 +2357,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2322,7 +2392,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2357,7 +2427,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -2427,7 +2497,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="44.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -2459,7 +2529,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2491,7 +2561,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2596,7 +2666,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2666,7 +2736,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2841,7 +2911,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -2876,7 +2946,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2911,7 +2981,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2946,7 +3016,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -2963,7 +3033,7 @@
         <v>78</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>215</v>
+        <v>313</v>
       </c>
       <c r="G26" t="s">
         <v>92</v>
@@ -2981,7 +3051,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2998,7 +3068,7 @@
         <v>179</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>251</v>
+        <v>312</v>
       </c>
       <c r="G27" t="s">
         <v>92</v>
@@ -3013,7 +3083,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -3030,7 +3100,7 @@
         <v>165</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>245</v>
+        <v>315</v>
       </c>
       <c r="G28" t="s">
         <v>92</v>
@@ -3048,7 +3118,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -3065,7 +3135,7 @@
         <v>183</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>253</v>
+        <v>319</v>
       </c>
       <c r="G29" t="s">
         <v>92</v>
@@ -3083,7 +3153,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -3100,7 +3170,7 @@
         <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>216</v>
+        <v>318</v>
       </c>
       <c r="G30" t="s">
         <v>92</v>
@@ -3118,7 +3188,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -3135,7 +3205,7 @@
         <v>188</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>255</v>
+        <v>317</v>
       </c>
       <c r="G31" t="s">
         <v>92</v>
@@ -3153,7 +3223,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -3170,7 +3240,7 @@
         <v>170</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>247</v>
+        <v>316</v>
       </c>
       <c r="G32" t="s">
         <v>92</v>
@@ -3188,7 +3258,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -3205,7 +3275,7 @@
         <v>265</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>257</v>
+        <v>320</v>
       </c>
       <c r="G33" t="s">
         <v>92</v>
@@ -3223,7 +3293,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -3240,7 +3310,7 @@
         <v>266</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>259</v>
+        <v>314</v>
       </c>
       <c r="G34" t="s">
         <v>92</v>
@@ -3258,7 +3328,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -3275,7 +3345,7 @@
         <v>264</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>249</v>
+        <v>321</v>
       </c>
       <c r="G35" t="s">
         <v>92</v>
@@ -3294,13 +3364,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K35" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="H"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K35" xr:uid="{5702DBC6-33CB-487C-91B4-3C688E088956}"/>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:I4" xr:uid="{AD8D866F-2288-4C7D-9144-AB3ACAF95A3B}">
       <formula1>Type</formula1>

</xml_diff>